<commit_message>
Updates to tables to make headings bold and lines consistent, inserted groundsbot logo.
</commit_message>
<xml_diff>
--- a/mechanical/development/platform/platform bom.xlsx
+++ b/mechanical/development/platform/platform bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Part No</t>
   </si>
@@ -99,31 +99,37 @@
     <t>S-5210-PRB</t>
   </si>
   <si>
-    <t>ARK-2250L-9S51</t>
-  </si>
-  <si>
-    <t>Advantech</t>
-  </si>
-  <si>
-    <t>Intel 6th Gen i3 Embedded PC</t>
-  </si>
-  <si>
     <t>Misc Item Extrusion</t>
   </si>
   <si>
     <t>Item</t>
   </si>
   <si>
-    <t>Misc</t>
-  </si>
-  <si>
-    <t>http://buy.advantech.com/Embedded-Computers/Embedded-Series-By-Processor-Intel-i-Series-Processor/ARK-2250L-9S51/system-21865.htm</t>
-  </si>
-  <si>
     <t>Misc Fasteners</t>
   </si>
   <si>
     <t>McMaster-Carr</t>
+  </si>
+  <si>
+    <t>https://www.lithiumion-batteries.com/products/lithium-ion-chargers/24v-lithium-ion-battery-chargers/dual-bank-6-amp-charger.php</t>
+  </si>
+  <si>
+    <t>Battery Charger</t>
+  </si>
+  <si>
+    <t>Misc Mechanical Parts</t>
+  </si>
+  <si>
+    <t>Misc Electrical Parts</t>
+  </si>
+  <si>
+    <t>NVIDIA Jetson TX2 Dev Kit</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/NVIDIA-Jetson-TX2-Development-Kit/dp/B06XPFH939</t>
+  </si>
+  <si>
+    <t>DP-RS2</t>
   </si>
 </sst>
 </file>
@@ -133,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,7 +155,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -192,16 +213,18 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -484,19 +507,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A2209" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="7" width="11.28515625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -526,236 +551,317 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>897</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
         <f>E2*D2</f>
         <v>897</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="7">
         <v>31</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>699.98</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
-        <f t="shared" ref="F3:F10" si="0">E3*D3</f>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F11" si="0">E3*D3</f>
         <v>699.98</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="7">
         <v>18</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5">
+        <v>164.99</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="0"/>
+        <v>164.99</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="5">
         <v>328.91</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
         <f t="shared" si="0"/>
         <v>328.91</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G5" s="7">
         <v>0.5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D6" s="5">
         <v>148.80000000000001</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>148.80000000000001</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G6" s="7">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D7" s="5">
         <v>67.63</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>67.63</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G7" s="7">
         <v>12</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5">
+        <v>560</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="0"/>
+        <v>560</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5">
         <v>1100</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
-      <c r="G7" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="G9" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3">
-        <v>300</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5">
+        <v>500</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="G8" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="3">
-        <v>250</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="G9" s="6">
+        <v>500</v>
+      </c>
+      <c r="G10" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F10" s="4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12" s="4">
-        <f>SUM(F2:F10)</f>
-        <v>3792.32</v>
-      </c>
-      <c r="G12">
-        <f>SUM(G2:G10)</f>
-        <v>85</v>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="6">
+        <f>SUM(F2:F11)</f>
+        <v>4467.3100000000004</v>
+      </c>
+      <c r="G13" s="3">
+        <f>SUM(G2:G11)</f>
+        <v>85.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="3">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="3">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="3">
+        <f>SUM(F16:F25)</f>
+        <v>4375</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1"/>
     <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>